<commit_message>
add Tcs related to Car_SRS_02
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_SearchTCs.xlsx
+++ b/Car_TestCases/Car_SearchTCs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,9 +13,131 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+  <si>
+    <t>Test case ID</t>
+  </si>
+  <si>
+    <t>Related Requirement</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>Attachements</t>
+  </si>
+  <si>
+    <t>Designed by</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Bug ID</t>
+  </si>
+  <si>
+    <t>Reviewed by</t>
+  </si>
+  <si>
+    <t>Car_SRS_02</t>
+  </si>
+  <si>
+    <t>Car_SearchTC_01</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Validate that the guest can search for cars colors by choosing the desired color from the colors drop down list</t>
+  </si>
+  <si>
+    <t>Don't login to the website, use an unregistered user</t>
+  </si>
+  <si>
+    <t>1. Navigate to car connect website "http://localhost:8080/Car_implementation/"
+2. In the home page, Check that the colors drop down list is set to " All colors" and the cars viewed in the home page have different colors</t>
+  </si>
+  <si>
+    <t>the colors drop down list is set to " All colors" and the cars viewed in the home page have different colors</t>
+  </si>
+  <si>
+    <t>Jannat</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the guest after navigation to the website, he will found a list of cars with different colors and the colors drop down list is set to " All colors" </t>
+  </si>
+  <si>
+    <t>1. Navigate to car connect website "http://localhost:8080/Car_implementation/"
+2. In the home page,click the colors drop down list
+3. choose "Gray"</t>
+  </si>
+  <si>
+    <t>All gray cars in the database are viewed in the search result page</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>Validate that the search result is the result of searching the whole database not by just filtering the exsiting cars viewed in the page</t>
+  </si>
+  <si>
+    <t>1. Navigate to car connect website "http://localhost:8080/Car_implementation/"
+2. In the home page,click the colors drop down list
+3. choose "Gray"
+4. After checking the gray cars, click on the drop down list again
+5. choose "red"</t>
+  </si>
+  <si>
+    <t>All red cars in the database are viewed in the search result page</t>
+  </si>
+  <si>
+    <t>Validate that If the user click back after choosing a color, the viewed cars and the dropdown list will be rolled back to their previous state</t>
+  </si>
+  <si>
+    <t>1. Navigate to car connect website "http://localhost:8080/Car_implementation/"
+2. In the home page,click the colors drop down list
+3. choose "Gray"
+4. After checking the gray cars, click on the drop down list again
+5. choose "red"
+6. click back and check on the results viewed and the drop down list</t>
+  </si>
+  <si>
+    <t>All gray cars in the database are viewed in the search result page again and the colors down down list value is set to " Gray"</t>
+  </si>
+  <si>
+    <t>Car_SearchTC_02</t>
+  </si>
+  <si>
+    <t>Car_SearchTC_03</t>
+  </si>
+  <si>
+    <t>Car_SearchTC_04</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,13 +145,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -44,14 +185,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +256,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +291,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +499,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="142.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="27.42578125" style="2"/>
+    <col min="7" max="7" width="42.140625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="27.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the bugs IDs
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_SearchTCs.xlsx
+++ b/Car_TestCases/Car_SearchTCs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="122">
   <si>
     <t>Test case ID</t>
   </si>
@@ -407,6 +407,27 @@
   </si>
   <si>
     <t>Car_SearchTC_26</t>
+  </si>
+  <si>
+    <t>Car_SearchBug_02</t>
+  </si>
+  <si>
+    <t>Car_SearchBug_01</t>
+  </si>
+  <si>
+    <t>Car_SearchBug_03</t>
+  </si>
+  <si>
+    <t>Car_SearchBug_04</t>
+  </si>
+  <si>
+    <t>Car_SearchBug_05</t>
+  </si>
+  <si>
+    <t>Car_SearchBug_06</t>
+  </si>
+  <si>
+    <t>Car_SearchBug_07</t>
   </si>
 </sst>
 </file>
@@ -469,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -482,6 +503,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -789,7 +813,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="142.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -867,6 +893,9 @@
       <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="L2" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -954,6 +983,9 @@
       <c r="K5" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="L5" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1039,7 +1071,7 @@
         <v>20</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1067,6 +1099,9 @@
       <c r="K9" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="L9" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1096,6 +1131,9 @@
       <c r="K10" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="L10" s="5" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1154,6 +1192,9 @@
       <c r="K12" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="L12" s="5" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1268,10 +1309,10 @@
         <v>20</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>104</v>
       </c>
@@ -1303,7 +1344,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>105</v>
       </c>
@@ -1335,7 +1376,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>106</v>
       </c>
@@ -1366,8 +1407,11 @@
       <c r="K19" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>107</v>
       </c>
@@ -1399,7 +1443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>108</v>
       </c>
@@ -1431,7 +1475,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>109</v>
       </c>
@@ -1460,10 +1504,10 @@
         <v>20</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>110</v>
       </c>
@@ -1495,7 +1539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>111</v>
       </c>
@@ -1527,7 +1571,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>112</v>
       </c>
@@ -1558,8 +1602,11 @@
       <c r="K25" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>113</v>
       </c>
@@ -1591,7 +1638,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Review some test cases
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_SearchTCs.xlsx
+++ b/Car_TestCases/Car_SearchTCs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="123">
   <si>
     <t>Test case ID</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>Car_SearchBug_07</t>
+  </si>
+  <si>
+    <t>Fatma</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="142.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -896,6 +899,9 @@
       <c r="L2" s="5" t="s">
         <v>116</v>
       </c>
+      <c r="M2" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -925,6 +931,9 @@
       <c r="K3" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="M3" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -954,6 +963,9 @@
       <c r="K4" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="M4" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -985,6 +997,9 @@
       </c>
       <c r="L5" s="5" t="s">
         <v>115</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="168" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>